<commit_message>
Booking fee at prices
</commit_message>
<xml_diff>
--- a/app/templates/report/precios.xlsx
+++ b/app/templates/report/precios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694CFA76-8275-401E-B2EE-CD75C2462882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB578C9-28F7-4C02-9139-58010AE0DEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Año</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Building.Name</t>
+  </si>
+  <si>
+    <t>Booking fee</t>
+  </si>
+  <si>
+    <t>Booking_fee</t>
   </si>
 </sst>
 </file>
@@ -237,7 +243,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,6 +265,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -643,7 +650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -656,11 +663,11 @@
     <col min="5" max="5" width="24.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="17.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="24.85546875" style="2"/>
+    <col min="8" max="17" width="17.7109375" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="24.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -703,8 +710,11 @@
       <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -749,8 +759,11 @@
       <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="Q2" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -767,12 +780,13 @@
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
-      <c r="Q3" s="10" t="str">
+      <c r="Q3" s="11"/>
+      <c r="R3" s="10" t="str">
         <f>A3&amp;B3&amp;D3&amp;F3</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A2:M3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>